<commit_message>
scripts edited to work for Shiny
</commit_message>
<xml_diff>
--- a/data/ASP_input_parameters_german.xlsx
+++ b/data/ASP_input_parameters_german.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb83dfbf15e16b51/UNI/Bonn/HortiBonn/4.Asparagus/Climate_Impact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\Onion_DA_model\climate_Impact\Climate_Impact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{C0D80277-9E22-9B4E-9CB5-B67ECAE68C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{963CC2E3-1149-7D46-AC26-ED15F8365B12}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD6C02E-2A3C-4AC2-B3AA-CBC0948B9B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="328">
   <si>
     <t>variable</t>
   </si>
@@ -958,6 +958,72 @@
   </si>
   <si>
     <t>Spagelbauer;Datenanalyst;Market analyst;Policy-maker</t>
+  </si>
+  <si>
+    <t>rain_window_days_sowing_p</t>
+  </si>
+  <si>
+    <t>Rainfall window before sowing [days]</t>
+  </si>
+  <si>
+    <t>The number of days before sowing is considered for the rainfall accumulation check.</t>
+  </si>
+  <si>
+    <t>base_temp_p</t>
+  </si>
+  <si>
+    <t>Basisstemperatur [°C]</t>
+  </si>
+  <si>
+    <t>Temperature threshold for onion growth</t>
+  </si>
+  <si>
+    <t>leaf_area_em_per_plant_p</t>
+  </si>
+  <si>
+    <t>rh_drought_threshold_p</t>
+  </si>
+  <si>
+    <t>Blattfläche pro Pflanze Feldaufgang [cm²]</t>
+  </si>
+  <si>
+    <t>Blattfläche pro Pflanze während der Auflaufphase. [cm²]</t>
+  </si>
+  <si>
+    <t>Zwiebel Anbauberater; Datenanalyst</t>
+  </si>
+  <si>
+    <t>Blattfläche pro Pflanze vegetative Phase [cm²]</t>
+  </si>
+  <si>
+    <t>Blattflächenindex während der vegetativen Wachstumsphase. [cm²]</t>
+  </si>
+  <si>
+    <t>leaf_area_bl_per_plant_p</t>
+  </si>
+  <si>
+    <t>Blattfläche pro Pflanze Knollenbildungsphase [cm²]</t>
+  </si>
+  <si>
+    <t>Blattflächenindex während der Knollenbildungsphase. [cm²]</t>
+  </si>
+  <si>
+    <t>leaf_area_mt_per_plant_p</t>
+  </si>
+  <si>
+    <t>Blattfläche pro Pflanze Abreifephase [cm²]</t>
+  </si>
+  <si>
+    <t>Blattflächenindex während der Reifephase. [cm²]</t>
+  </si>
+  <si>
+    <t>Datenanalyst; Zwiebel Anbauberater; Zwiebelbauer</t>
+  </si>
+  <si>
+    <t>impact_rh_drought_t</t>
+  </si>
+  <si>
+    <t>leaf_area_veg_per_plant_p</t>
   </si>
 </sst>
 </file>
@@ -967,7 +1033,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1065,10 +1131,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1356,15 +1418,15 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="73.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1372,7 +1434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1380,7 +1442,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1388,7 +1450,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1396,7 +1458,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1404,7 +1466,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -1412,7 +1474,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1420,7 +1482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1428,14 +1490,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
@@ -1446,22 +1508,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92018703-4177-49D8-B09E-62560F009CDF}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="66.83203125" customWidth="1"/>
-    <col min="10" max="10" width="70.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="66.77734375" customWidth="1"/>
+    <col min="10" max="10" width="70.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1496,7 +1558,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
@@ -1531,7 +1593,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -1566,7 +1628,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1601,7 +1663,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -1636,7 +1698,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -1671,7 +1733,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>297</v>
       </c>
@@ -1703,7 +1765,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>237</v>
       </c>
@@ -1738,7 +1800,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>298</v>
       </c>
@@ -1770,7 +1832,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>244</v>
       </c>
@@ -1805,7 +1867,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>247</v>
       </c>
@@ -1840,7 +1902,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>251</v>
       </c>
@@ -1875,7 +1937,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>254</v>
       </c>
@@ -1910,7 +1972,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -1945,7 +2007,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>261</v>
       </c>
@@ -1980,7 +2042,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>265</v>
       </c>
@@ -2012,6 +2074,38 @@
         <v>234</v>
       </c>
       <c r="K16" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>310</v>
+      </c>
+      <c r="G17" t="s">
+        <v>311</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17">
+        <v>0.1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>234</v>
+      </c>
+      <c r="K17" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2026,26 +2120,26 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="79" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="53.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="1"/>
+    <col min="12" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2080,7 +2174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
@@ -2115,7 +2209,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -2150,7 +2244,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
         <v>33</v>
       </c>
@@ -2185,7 +2279,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="5" t="s">
         <v>34</v>
       </c>
@@ -2220,37 +2314,37 @@
         <v>301</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="J6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="J7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="J8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="J10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="J12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="J15"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2259,7 +2353,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.6">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2268,7 +2362,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.6">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2291,19 +2385,19 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="48.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.77734375" style="1"/>
     <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.77734375" style="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="70.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="1"/>
+    <col min="9" max="9" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="70.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2432,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -2373,7 +2467,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -2408,7 +2502,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -2443,7 +2537,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -2478,10 +2572,10 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="F12" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2490,7 +2584,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15.6">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2499,7 +2593,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.6">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2515,24 +2609,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49756CD-7B89-4299-B487-83FA9AC75873}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="60.1640625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="60.109375" style="1" customWidth="1"/>
+    <col min="2" max="5" width="8.77734375" style="1"/>
     <col min="6" max="6" width="51.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="85.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="85.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.77734375" style="1"/>
     <col min="10" max="10" width="40.33203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="1"/>
+    <col min="11" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2567,7 +2661,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="F2" s="3" t="s">
         <v>80</v>
       </c>
@@ -2576,7 +2670,7 @@
       </c>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -2611,7 +2705,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -2646,7 +2740,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -2679,7 +2773,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -2712,14 +2806,14 @@
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="H7" s="1" t="s">
         <v>79</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="F8" s="3" t="s">
         <v>92</v>
       </c>
@@ -2728,7 +2822,7 @@
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -2763,7 +2857,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -2798,7 +2892,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -2831,7 +2925,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>299</v>
       </c>
@@ -2864,13 +2958,13 @@
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="H13" s="1" t="s">
         <v>79</v>
       </c>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="F14" s="9" t="s">
         <v>104</v>
       </c>
@@ -2879,7 +2973,7 @@
       </c>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -2911,27 +3005,27 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>313</v>
       </c>
       <c r="B16">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="C16">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
@@ -2940,37 +3034,39 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>234</v>
+        <v>325</v>
       </c>
       <c r="K16" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B17">
-        <v>0.5</v>
+        <v>24</v>
       </c>
       <c r="C17">
-        <v>0.6</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17"/>
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
       <c r="F17" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H17" t="s">
         <v>19</v>
       </c>
       <c r="I17">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J17" t="s">
         <v>234</v>
@@ -2979,31 +3075,31 @@
         <v>302</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="C18">
         <v>0.6</v>
-      </c>
-      <c r="C18">
-        <v>0.7</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18"/>
       <c r="F18" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H18" t="s">
         <v>19</v>
       </c>
       <c r="I18">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="J18" t="s">
         <v>234</v>
@@ -3012,60 +3108,58 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>326</v>
       </c>
       <c r="B19">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="C19">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
-        <v>97</v>
-      </c>
+      <c r="E19"/>
       <c r="F19" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H19" t="s">
         <v>19</v>
       </c>
       <c r="I19">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J19" t="s">
-        <v>234</v>
+        <v>325</v>
       </c>
       <c r="K19" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B20">
         <v>0.6</v>
       </c>
       <c r="C20">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
       <c r="E20"/>
       <c r="F20" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H20" t="s">
         <v>19</v>
@@ -3080,36 +3174,75 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21">
+        <v>0.2</v>
+      </c>
+      <c r="C21">
+        <v>0.3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21">
+        <v>0.5</v>
+      </c>
+      <c r="J21" t="s">
+        <v>234</v>
+      </c>
+      <c r="K21" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22">
+        <v>0.6</v>
+      </c>
+      <c r="C22">
+        <v>0.9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
       <c r="E22"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F22" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22">
+        <v>0.05</v>
+      </c>
+      <c r="J22" t="s">
+        <v>234</v>
+      </c>
+      <c r="K22" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -3122,7 +3255,7 @@
       <c r="J24"/>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -3135,7 +3268,7 @@
       <c r="J25"/>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -3148,7 +3281,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -3161,8 +3294,34 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F30"/>
+    <row r="28" spans="1:11">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="F32"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3174,22 +3333,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8485F19-4118-CA49-B5A5-49D6574876CF}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="60.1640625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="60.109375" style="1" customWidth="1"/>
+    <col min="2" max="5" width="8.77734375" style="1"/>
     <col min="6" max="6" width="51.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="85.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="1"/>
-    <col min="10" max="10" width="69.83203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="85.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.77734375" style="1"/>
+    <col min="10" max="10" width="69.77734375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" customFormat="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3224,7 +3383,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="F2" s="3" t="s">
@@ -3234,7 +3393,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>268</v>
       </c>
@@ -3269,7 +3428,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -3304,7 +3463,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>243</v>
       </c>
@@ -3339,7 +3498,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>271</v>
       </c>
@@ -3372,7 +3531,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -3405,7 +3564,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>134</v>
       </c>
@@ -3438,13 +3597,13 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="H9" s="1" t="s">
         <v>79</v>
       </c>
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="F10" s="10" t="s">
         <v>137</v>
       </c>
@@ -3453,7 +3612,7 @@
       </c>
       <c r="J10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>275</v>
       </c>
@@ -3488,7 +3647,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -3523,7 +3682,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>144</v>
       </c>
@@ -3558,7 +3717,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>277</v>
       </c>
@@ -3593,7 +3752,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -3626,7 +3785,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -3659,13 +3818,13 @@
         <v>302</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="H17" s="1" t="s">
         <v>79</v>
       </c>
       <c r="J17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="F18" s="9" t="s">
         <v>149</v>
       </c>
@@ -3674,7 +3833,7 @@
       </c>
       <c r="J18"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>281</v>
       </c>
@@ -3709,7 +3868,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>282</v>
       </c>
@@ -3744,7 +3903,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>283</v>
       </c>
@@ -3779,7 +3938,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>284</v>
       </c>
@@ -3814,7 +3973,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>152</v>
       </c>
@@ -3847,7 +4006,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>159</v>
       </c>
@@ -3880,7 +4039,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -3894,7 +4053,7 @@
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -3910,7 +4069,7 @@
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>287</v>
       </c>
@@ -3945,7 +4104,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>163</v>
       </c>
@@ -3980,7 +4139,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -4015,7 +4174,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>290</v>
       </c>
@@ -4048,7 +4207,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -4081,7 +4240,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>174</v>
       </c>
@@ -4114,7 +4273,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -4125,7 +4284,7 @@
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -4137,7 +4296,7 @@
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -4149,7 +4308,7 @@
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -4161,7 +4320,7 @@
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -4173,7 +4332,7 @@
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -4185,7 +4344,7 @@
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -4197,7 +4356,7 @@
       <c r="I39"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -4209,7 +4368,7 @@
       <c r="I40"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -4220,7 +4379,7 @@
       <c r="I41"/>
       <c r="J41"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -4232,7 +4391,7 @@
       <c r="I42"/>
       <c r="J42"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -4244,7 +4403,7 @@
       <c r="I43"/>
       <c r="J43"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -4256,7 +4415,7 @@
       <c r="I44"/>
       <c r="J44"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -4268,7 +4427,7 @@
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -4280,7 +4439,7 @@
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -4292,7 +4451,7 @@
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -4312,24 +4471,24 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E27EF3F-1977-4DFD-AB2B-D5DA3F473BBD}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="30.109375" style="1" customWidth="1"/>
+    <col min="2" max="5" width="8.77734375" style="1"/>
     <col min="6" max="6" width="45.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="66.33203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="1"/>
-    <col min="10" max="10" width="40.83203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="1"/>
+    <col min="8" max="9" width="8.77734375" style="1"/>
+    <col min="10" max="10" width="40.77734375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" customFormat="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4364,7 +4523,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -4399,7 +4558,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -4434,7 +4593,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -4469,7 +4628,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -4504,7 +4663,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -4539,7 +4698,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>195</v>
       </c>
@@ -4572,7 +4731,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>198</v>
       </c>
@@ -4605,7 +4764,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>201</v>
       </c>
@@ -4638,7 +4797,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>204</v>
       </c>
@@ -4671,7 +4830,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -4704,7 +4863,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>210</v>
       </c>
@@ -4737,7 +4896,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>213</v>
       </c>
@@ -4772,7 +4931,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>216</v>
       </c>
@@ -4807,7 +4966,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>219</v>
       </c>
@@ -4842,7 +5001,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>222</v>
       </c>
@@ -4877,7 +5036,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>225</v>
       </c>
@@ -4912,7 +5071,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>228</v>
       </c>
@@ -4947,7 +5106,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>231</v>
       </c>
@@ -4981,6 +5140,130 @@
       <c r="K19" s="1" t="s">
         <v>302</v>
       </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>312</v>
+      </c>
+      <c r="B20">
+        <v>0.2</v>
+      </c>
+      <c r="C20">
+        <v>0.4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <v>0.1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>316</v>
+      </c>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>327</v>
+      </c>
+      <c r="B21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C21">
+        <v>1.3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21">
+        <v>0.1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>316</v>
+      </c>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>319</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22">
+        <v>0.1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>316</v>
+      </c>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>322</v>
+      </c>
+      <c r="B23">
+        <v>1.4</v>
+      </c>
+      <c r="C23">
+        <v>1.6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23">
+        <v>0.1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>316</v>
+      </c>
+      <c r="K23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4992,24 +5275,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E46615A-8238-4E62-BD61-353FBA21321A}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="136" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="34.109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="1"/>
     <col min="6" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="7" width="52" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="1"/>
-    <col min="10" max="10" width="70.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="1"/>
+    <col min="8" max="9" width="8.77734375" style="1"/>
+    <col min="10" max="10" width="70.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5044,7 +5327,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5082,7 +5365,7 @@
       <c r="M2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>293</v>
       </c>
@@ -5115,7 +5398,42 @@
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>307</v>
+      </c>
+      <c r="G4" t="s">
+        <v>308</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>304</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5124,7 +5442,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="15.6">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -5133,7 +5451,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="15.6">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -5142,7 +5460,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="15.6">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -5151,7 +5469,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.6">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -5160,7 +5478,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.6">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -5169,7 +5487,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.6">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -5178,19 +5496,19 @@
       <c r="F19" s="6"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="F28" s="3"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:6">
       <c r="F36" s="3"/>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:6">
       <c r="F42" s="3"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:6">
       <c r="F49" s="3"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:6">
       <c r="F54" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
loading animation added, input file upadte, fig titile subtitle description via add_meta()
</commit_message>
<xml_diff>
--- a/data/ASP_input_parameters_german.xlsx
+++ b/data/ASP_input_parameters_german.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\Onion_DA_model\climate_Impact\Climate_Impact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD6C02E-2A3C-4AC2-B3AA-CBC0948B9B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0633D08F-455E-43D6-8379-BE490CFB02F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="316">
   <si>
     <t>variable</t>
   </si>
@@ -625,42 +625,6 @@
   </si>
   <si>
     <t>Biomasseproduktion pro Einheit eingestrahlter und genutzter Strahlung (g/MJ).</t>
-  </si>
-  <si>
-    <t>LAI_emergence_p</t>
-  </si>
-  <si>
-    <t>Blattflächenindex Feldaufgang</t>
-  </si>
-  <si>
-    <t>Blattflächenindex während der Auflaufphase.</t>
-  </si>
-  <si>
-    <t>LAI_veg_p</t>
-  </si>
-  <si>
-    <t>Blattflächenindex vegetative Phase</t>
-  </si>
-  <si>
-    <t>Blattflächenindex während der vegetativen Wachstumsphase.</t>
-  </si>
-  <si>
-    <t>LAI_bulbing_p</t>
-  </si>
-  <si>
-    <t>Blattflächenindex Knollenbildungsphase</t>
-  </si>
-  <si>
-    <t>Blattflächenindex während der Knollenbildungsphase.</t>
-  </si>
-  <si>
-    <t>LAI_maturation_p</t>
-  </si>
-  <si>
-    <t>Blattflächenindex Abreifephase</t>
-  </si>
-  <si>
-    <t>Blattflächenindex während der Reifephase.</t>
   </si>
   <si>
     <t>Krs_c</t>
@@ -1587,10 +1551,10 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="K2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1622,10 +1586,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="K3" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1657,10 +1621,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="K4" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1">
@@ -1692,10 +1656,10 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K5" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1">
@@ -1727,15 +1691,15 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K6" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="B7">
         <v>0.65</v>
@@ -1747,10 +1711,10 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="G7" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
@@ -1759,15 +1723,15 @@
         <v>0.1</v>
       </c>
       <c r="J7" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K7" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B8">
         <v>700000</v>
@@ -1779,13 +1743,13 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="F8" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G8" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
@@ -1794,15 +1758,15 @@
         <v>0.1</v>
       </c>
       <c r="J8" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K8" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B9">
         <v>0.88</v>
@@ -1814,10 +1778,10 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="G9" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="H9" t="s">
         <v>19</v>
@@ -1826,15 +1790,15 @@
         <v>0.05</v>
       </c>
       <c r="J9" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K9" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1849,10 +1813,10 @@
         <v>97</v>
       </c>
       <c r="F10" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="G10" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
@@ -1861,15 +1825,15 @@
         <v>0.5</v>
       </c>
       <c r="J10" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K10" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1881,13 +1845,13 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="F11" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="G11" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
@@ -1896,15 +1860,15 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K11" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -1916,13 +1880,13 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="F12" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="G12" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
@@ -1931,15 +1895,15 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K12" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1951,13 +1915,13 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="F13" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="G13" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="H13" t="s">
         <v>19</v>
@@ -1966,15 +1930,15 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K13" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1986,13 +1950,13 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G14" t="s">
         <v>248</v>
-      </c>
-      <c r="F14" t="s">
-        <v>259</v>
-      </c>
-      <c r="G14" t="s">
-        <v>260</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -2001,15 +1965,15 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K14" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B15">
         <v>45</v>
@@ -2021,13 +1985,13 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="F15" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="G15" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
@@ -2036,15 +2000,15 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K15" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="B16">
         <v>100</v>
@@ -2056,13 +2020,13 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="F16" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="G16" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
@@ -2071,15 +2035,15 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K16" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2091,10 +2055,10 @@
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="G17" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="H17" t="s">
         <v>19</v>
@@ -2103,10 +2067,10 @@
         <v>0.1</v>
       </c>
       <c r="J17" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K17" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2203,10 +2167,10 @@
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2238,10 +2202,10 @@
         <v>0.1</v>
       </c>
       <c r="J3" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K3" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2273,10 +2237,10 @@
         <v>0.1</v>
       </c>
       <c r="J4" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K4" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2308,10 +2272,10 @@
         <v>0.1</v>
       </c>
       <c r="J5" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K5" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2461,10 +2425,10 @@
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2496,10 +2460,10 @@
         <v>0.1</v>
       </c>
       <c r="J3" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K3" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2531,10 +2495,10 @@
         <v>0.1</v>
       </c>
       <c r="J4" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K4" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2566,10 +2530,10 @@
         <v>0.1</v>
       </c>
       <c r="J5" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="K5" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2611,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49756CD-7B89-4299-B487-83FA9AC75873}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2702,7 +2666,7 @@
         <v>76</v>
       </c>
       <c r="K3" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2737,12 +2701,12 @@
         <v>76</v>
       </c>
       <c r="K4" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="B5">
         <v>0.3</v>
@@ -2770,7 +2734,7 @@
         <v>77</v>
       </c>
       <c r="K5" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2803,7 +2767,7 @@
         <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2851,10 +2815,10 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K9" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2886,10 +2850,10 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K10" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2910,7 +2874,7 @@
         <v>101</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
@@ -2919,15 +2883,15 @@
         <v>0.1</v>
       </c>
       <c r="J11" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K11" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="B12">
         <v>0.5</v>
@@ -2952,10 +2916,10 @@
         <v>0.05</v>
       </c>
       <c r="J12" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K12" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -3002,12 +2966,12 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="B16">
         <v>85</v>
@@ -3034,10 +2998,10 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="K16" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -3069,10 +3033,10 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K17" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -3102,15 +3066,15 @@
         <v>0.1</v>
       </c>
       <c r="J18" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K18" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="B19">
         <v>0.5</v>
@@ -3135,10 +3099,10 @@
         <v>0.1</v>
       </c>
       <c r="J19" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="K19" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -3168,10 +3132,10 @@
         <v>0.05</v>
       </c>
       <c r="J20" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K20" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -3200,13 +3164,13 @@
         <v>19</v>
       </c>
       <c r="I21">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="J21" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K21" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -3236,10 +3200,10 @@
         <v>0.05</v>
       </c>
       <c r="J22" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K22" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -3395,7 +3359,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B3">
         <v>85</v>
@@ -3410,10 +3374,10 @@
         <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="G3" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -3422,10 +3386,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3457,15 +3421,15 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3492,15 +3456,15 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="B6">
         <v>0.4</v>
@@ -3513,10 +3477,10 @@
       </c>
       <c r="E6"/>
       <c r="F6" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="G6" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="H6" t="s">
         <v>19</v>
@@ -3525,10 +3489,10 @@
         <v>0.1</v>
       </c>
       <c r="J6" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3549,7 +3513,7 @@
         <v>128</v>
       </c>
       <c r="G7" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
@@ -3558,10 +3522,10 @@
         <v>0.1</v>
       </c>
       <c r="J7" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -3591,10 +3555,10 @@
         <v>0.05</v>
       </c>
       <c r="J8" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3614,7 +3578,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B11">
         <v>85</v>
@@ -3629,7 +3593,7 @@
         <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="G11" t="s">
         <v>138</v>
@@ -3641,10 +3605,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -3676,10 +3640,10 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -3711,15 +3675,15 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B14">
         <v>0.4</v>
@@ -3734,10 +3698,10 @@
         <v>78</v>
       </c>
       <c r="F14" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="G14" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -3746,10 +3710,10 @@
         <v>0.1</v>
       </c>
       <c r="J14" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -3770,7 +3734,7 @@
         <v>140</v>
       </c>
       <c r="G15" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
@@ -3779,10 +3743,10 @@
         <v>0.1</v>
       </c>
       <c r="J15" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -3812,10 +3776,10 @@
         <v>0.05</v>
       </c>
       <c r="J16" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -3835,7 +3799,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3862,15 +3826,15 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B20">
         <v>22</v>
@@ -3897,15 +3861,15 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -3932,15 +3896,15 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B22">
         <v>0.3</v>
@@ -3955,10 +3919,10 @@
         <v>78</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="H22" t="s">
         <v>19</v>
@@ -3967,10 +3931,10 @@
         <v>0.1</v>
       </c>
       <c r="J22" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -4000,10 +3964,10 @@
         <v>0.1</v>
       </c>
       <c r="J23" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -4033,10 +3997,10 @@
         <v>0.05</v>
       </c>
       <c r="J24" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -4071,7 +4035,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B27">
         <v>40</v>
@@ -4086,10 +4050,10 @@
         <v>78</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="H27" t="s">
         <v>19</v>
@@ -4098,10 +4062,10 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -4133,10 +4097,10 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -4168,15 +4132,15 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="B30">
         <v>0.3</v>
@@ -4201,10 +4165,10 @@
         <v>0.1</v>
       </c>
       <c r="J30" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -4234,10 +4198,10 @@
         <v>0.1</v>
       </c>
       <c r="J31" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -4267,10 +4231,10 @@
         <v>0.05</v>
       </c>
       <c r="J32" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -4471,10 +4435,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E27EF3F-1977-4DFD-AB2B-D5DA3F473BBD}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -4555,7 +4519,7 @@
         <v>177</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4590,7 +4554,7 @@
         <v>177</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4625,7 +4589,7 @@
         <v>177</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -4660,7 +4624,7 @@
         <v>177</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -4695,12 +4659,12 @@
         <v>177</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>300</v>
       </c>
       <c r="B7">
         <v>0.2</v>
@@ -4713,10 +4677,10 @@
       </c>
       <c r="E7"/>
       <c r="F7" s="8" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>197</v>
+        <v>303</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
@@ -4725,15 +4689,13 @@
         <v>0.1</v>
       </c>
       <c r="J7" t="s">
-        <v>177</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>302</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K7"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>315</v>
       </c>
       <c r="B8">
         <v>1.1000000000000001</v>
@@ -4746,10 +4708,10 @@
       </c>
       <c r="E8"/>
       <c r="F8" s="8" t="s">
-        <v>199</v>
+        <v>305</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>200</v>
+        <v>306</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
@@ -4758,15 +4720,13 @@
         <v>0.1</v>
       </c>
       <c r="J8" t="s">
-        <v>177</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>302</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K8"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>307</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -4779,10 +4739,10 @@
       </c>
       <c r="E9"/>
       <c r="F9" s="8" t="s">
-        <v>202</v>
+        <v>308</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>203</v>
+        <v>309</v>
       </c>
       <c r="H9" t="s">
         <v>19</v>
@@ -4791,15 +4751,13 @@
         <v>0.1</v>
       </c>
       <c r="J9" t="s">
-        <v>177</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>302</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K9"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>310</v>
       </c>
       <c r="B10">
         <v>1.4</v>
@@ -4812,10 +4770,10 @@
       </c>
       <c r="E10"/>
       <c r="F10" s="8" t="s">
-        <v>205</v>
+        <v>311</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>206</v>
+        <v>312</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
@@ -4824,15 +4782,13 @@
         <v>0.1</v>
       </c>
       <c r="J10" t="s">
-        <v>177</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>302</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="K10"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B11">
         <v>0.17</v>
@@ -4845,10 +4801,10 @@
       </c>
       <c r="E11"/>
       <c r="F11" s="8" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
@@ -4860,12 +4816,12 @@
         <v>76</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B12">
         <v>0.65</v>
@@ -4878,10 +4834,10 @@
       </c>
       <c r="E12"/>
       <c r="F12" s="8" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
@@ -4893,12 +4849,12 @@
         <v>76</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B13">
         <v>23</v>
@@ -4913,10 +4869,10 @@
         <v>97</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="H13" t="s">
         <v>19</v>
@@ -4928,12 +4884,12 @@
         <v>76</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -4948,10 +4904,10 @@
         <v>97</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -4963,12 +4919,12 @@
         <v>76</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B15">
         <v>34</v>
@@ -4983,10 +4939,10 @@
         <v>97</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
@@ -4998,12 +4954,12 @@
         <v>76</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -5018,10 +4974,10 @@
         <v>97</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
@@ -5033,12 +4989,12 @@
         <v>76</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="B17">
         <v>9</v>
@@ -5053,10 +5009,10 @@
         <v>78</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="H17" t="s">
         <v>19</v>
@@ -5068,12 +5024,12 @@
         <v>76</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5088,10 +5044,10 @@
         <v>78</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="H18" t="s">
         <v>19</v>
@@ -5103,12 +5059,12 @@
         <v>76</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="B19">
         <v>0.8</v>
@@ -5123,10 +5079,10 @@
         <v>78</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="H19" t="s">
         <v>19</v>
@@ -5138,132 +5094,8 @@
         <v>76</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
-        <v>312</v>
-      </c>
-      <c r="B20">
-        <v>0.2</v>
-      </c>
-      <c r="C20">
-        <v>0.4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20"/>
-      <c r="F20" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="H20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20">
-        <v>0.1</v>
-      </c>
-      <c r="J20" t="s">
-        <v>316</v>
-      </c>
-      <c r="K20"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>327</v>
-      </c>
-      <c r="B21">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C21">
-        <v>1.3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21"/>
-      <c r="F21" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="H21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21">
-        <v>0.1</v>
-      </c>
-      <c r="J21" t="s">
-        <v>316</v>
-      </c>
-      <c r="K21"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
-        <v>319</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22"/>
-      <c r="F22" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="H22" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22">
-        <v>0.1</v>
-      </c>
-      <c r="J22" t="s">
-        <v>316</v>
-      </c>
-      <c r="K22"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
-        <v>322</v>
-      </c>
-      <c r="B23">
-        <v>1.4</v>
-      </c>
-      <c r="C23">
-        <v>1.6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23"/>
-      <c r="F23" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="H23" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23">
-        <v>0.1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>316</v>
-      </c>
-      <c r="K23"/>
+        <v>290</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5356,10 +5188,10 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="K2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="L2"/>
       <c r="M2"/>
@@ -5367,7 +5199,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B3">
         <v>50.866</v>
@@ -5380,10 +5212,10 @@
       </c>
       <c r="E3"/>
       <c r="F3" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="G3" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -5392,15 +5224,15 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -5415,10 +5247,10 @@
         <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="G4" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
@@ -5427,10 +5259,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:14">

</xml_diff>